<commit_message>
update to indices results
</commit_message>
<xml_diff>
--- a/data/indices/NIFTY 100_gainers.xlsx
+++ b/data/indices/NIFTY 100_gainers.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H47"/>
+  <dimension ref="A1:I46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -471,6 +471,11 @@
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
+          <t>To Year High Profit</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
           <t>Total Year Up</t>
         </is>
       </c>
@@ -492,7 +497,7 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>7388</v>
+        <v>7284.45</v>
       </c>
       <c r="E2" t="n">
         <v>8345</v>
@@ -501,10 +506,13 @@
         <v>2955</v>
       </c>
       <c r="G2" t="n">
-        <v>11.46794487717195</v>
+        <v>12.70880766926303</v>
       </c>
       <c r="H2" t="n">
-        <v>150.0169204737733</v>
+        <v>14.55909505865234</v>
+      </c>
+      <c r="I2" t="n">
+        <v>146.5126903553299</v>
       </c>
     </row>
     <row r="3">
@@ -524,7 +532,7 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>279.9</v>
+        <v>272.55</v>
       </c>
       <c r="E3" t="n">
         <v>304.7</v>
@@ -533,10 +541,13 @@
         <v>121.6</v>
       </c>
       <c r="G3" t="n">
-        <v>8.13915326550706</v>
+        <v>10.55136199540531</v>
       </c>
       <c r="H3" t="n">
-        <v>130.1809210526316</v>
+        <v>11.79600073381031</v>
+      </c>
+      <c r="I3" t="n">
+        <v>124.1365131578947</v>
       </c>
     </row>
     <row r="4">
@@ -556,7 +567,7 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>3201.5</v>
+        <v>3180</v>
       </c>
       <c r="E4" t="n">
         <v>3237.05</v>
@@ -565,74 +576,83 @@
         <v>1575</v>
       </c>
       <c r="G4" t="n">
-        <v>1.098222146707661</v>
+        <v>1.762407129948573</v>
       </c>
       <c r="H4" t="n">
-        <v>103.2698412698413</v>
+        <v>1.794025157232704</v>
+      </c>
+      <c r="I4" t="n">
+        <v>101.9047619047619</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>INE205A01025</t>
+          <t>INE663F01024</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>VEDL</t>
+          <t>NAUKRI</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Diversified Metals</t>
+          <t>Internet &amp; Catalogue Retail</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>464.65</v>
+        <v>9085</v>
       </c>
       <c r="E5" t="n">
-        <v>526.95</v>
+        <v>9085</v>
       </c>
       <c r="F5" t="n">
-        <v>249.5</v>
+        <v>4862.2</v>
       </c>
       <c r="G5" t="n">
-        <v>11.82275358193379</v>
+        <v>0</v>
       </c>
       <c r="H5" t="n">
-        <v>86.23246492985972</v>
+        <v>0</v>
+      </c>
+      <c r="I5" t="n">
+        <v>86.8495742667928</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>INE663F01024</t>
+          <t>INE205A01025</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>NAUKRI</t>
+          <t>VEDL</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Internet &amp; Catalogue Retail</t>
+          <t>Diversified Metals</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>8965</v>
+        <v>457.35</v>
       </c>
       <c r="E6" t="n">
-        <v>9040</v>
+        <v>526.95</v>
       </c>
       <c r="F6" t="n">
-        <v>4862.2</v>
+        <v>249.5</v>
       </c>
       <c r="G6" t="n">
-        <v>0.8296460176991149</v>
+        <v>13.20808425846854</v>
       </c>
       <c r="H6" t="n">
-        <v>84.38155567438608</v>
+        <v>15.21810429649067</v>
+      </c>
+      <c r="I6" t="n">
+        <v>83.30661322645292</v>
       </c>
     </row>
     <row r="7">
@@ -652,7 +672,7 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>6064</v>
+        <v>6042</v>
       </c>
       <c r="E7" t="n">
         <v>6285.45</v>
@@ -661,10 +681,13 @@
         <v>3350</v>
       </c>
       <c r="G7" t="n">
-        <v>3.523216317049693</v>
+        <v>3.87323103357754</v>
       </c>
       <c r="H7" t="n">
-        <v>81.01492537313433</v>
+        <v>4.029294935451833</v>
+      </c>
+      <c r="I7" t="n">
+        <v>80.35820895522387</v>
       </c>
     </row>
     <row r="8">
@@ -684,7 +707,7 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>295.1</v>
+        <v>291.95</v>
       </c>
       <c r="E8" t="n">
         <v>340.5</v>
@@ -693,10 +716,13 @@
         <v>171.75</v>
       </c>
       <c r="G8" t="n">
-        <v>13.33333333333333</v>
+        <v>14.25844346549193</v>
       </c>
       <c r="H8" t="n">
-        <v>71.81950509461427</v>
+        <v>16.62955985613976</v>
+      </c>
+      <c r="I8" t="n">
+        <v>69.98544395924309</v>
       </c>
     </row>
     <row r="9">
@@ -716,7 +742,7 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>6620</v>
+        <v>6610</v>
       </c>
       <c r="E9" t="n">
         <v>8129.9</v>
@@ -725,10 +751,13 @@
         <v>3965</v>
       </c>
       <c r="G9" t="n">
-        <v>18.57218415970676</v>
+        <v>18.69518690266793</v>
       </c>
       <c r="H9" t="n">
-        <v>66.9609079445145</v>
+        <v>22.99394856278365</v>
+      </c>
+      <c r="I9" t="n">
+        <v>66.70870113493064</v>
       </c>
     </row>
     <row r="10">
@@ -748,7 +777,7 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>1677.6</v>
+        <v>1680</v>
       </c>
       <c r="E10" t="n">
         <v>1700</v>
@@ -757,138 +786,153 @@
         <v>1054.7</v>
       </c>
       <c r="G10" t="n">
-        <v>1.317647058823535</v>
+        <v>1.17647058823529</v>
       </c>
       <c r="H10" t="n">
-        <v>59.05944818431781</v>
+        <v>1.190476190476186</v>
+      </c>
+      <c r="I10" t="n">
+        <v>59.28700104295059</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>INE775A01035</t>
+          <t>INE860A01027</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>MOTHERSON</t>
+          <t>HCLTECH</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Auto Components &amp; Equipments</t>
+          <t>Computers - Software &amp; Consulting</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>160.83</v>
+        <v>1943</v>
       </c>
       <c r="E11" t="n">
-        <v>216.99</v>
+        <v>1992.1</v>
       </c>
       <c r="F11" t="n">
-        <v>101.35</v>
+        <v>1235</v>
       </c>
       <c r="G11" t="n">
-        <v>25.88137702198258</v>
+        <v>2.464735706038845</v>
       </c>
       <c r="H11" t="n">
-        <v>58.68771583621118</v>
+        <v>2.527020072053521</v>
+      </c>
+      <c r="I11" t="n">
+        <v>57.32793522267205</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>INE860A01027</t>
+          <t>INE775A01035</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>HCLTECH</t>
+          <t>MOTHERSON</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Computers - Software &amp; Consulting</t>
+          <t>Auto Components &amp; Equipments</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>1955.55</v>
+        <v>159.45</v>
       </c>
       <c r="E12" t="n">
-        <v>1992.1</v>
+        <v>216.99</v>
       </c>
       <c r="F12" t="n">
-        <v>1235</v>
+        <v>101.35</v>
       </c>
       <c r="G12" t="n">
-        <v>1.834747251643987</v>
+        <v>26.51735103000139</v>
       </c>
       <c r="H12" t="n">
-        <v>58.34412955465586</v>
+        <v>36.08654750705551</v>
+      </c>
+      <c r="I12" t="n">
+        <v>57.32609768130241</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>INE117A01022</t>
+          <t>INE646L01027</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>ABB</t>
+          <t>INDIGO</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Heavy Electrical Equipment</t>
+          <t>Airline</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>6840.2</v>
+        <v>4472.5</v>
       </c>
       <c r="E13" t="n">
-        <v>9149.950000000001</v>
+        <v>5035</v>
       </c>
       <c r="F13" t="n">
-        <v>4340.3</v>
+        <v>2847</v>
       </c>
       <c r="G13" t="n">
-        <v>25.24330734047728</v>
+        <v>11.17179741807348</v>
       </c>
       <c r="H13" t="n">
-        <v>57.59740110130635</v>
+        <v>12.5768585802124</v>
+      </c>
+      <c r="I13" t="n">
+        <v>57.09518791710573</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>INE646L01027</t>
+          <t>INE117A01022</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>INDIGO</t>
+          <t>ABB</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Airline</t>
+          <t>Heavy Electrical Equipment</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>4476.5</v>
+        <v>6782</v>
       </c>
       <c r="E14" t="n">
-        <v>5035</v>
+        <v>9149.950000000001</v>
       </c>
       <c r="F14" t="n">
-        <v>2847</v>
+        <v>4340.3</v>
       </c>
       <c r="G14" t="n">
-        <v>11.09235352532274</v>
+        <v>25.87937639003492</v>
       </c>
       <c r="H14" t="n">
-        <v>57.23568668774148</v>
+        <v>34.91521675022118</v>
+      </c>
+      <c r="I14" t="n">
+        <v>56.25647996682257</v>
       </c>
     </row>
     <row r="15">
@@ -908,7 +952,7 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>1602.55</v>
+        <v>1594</v>
       </c>
       <c r="E15" t="n">
         <v>1779</v>
@@ -917,10 +961,13 @@
         <v>1021.35</v>
       </c>
       <c r="G15" t="n">
-        <v>9.918493535694218</v>
+        <v>10.3991006183249</v>
       </c>
       <c r="H15" t="n">
-        <v>56.90507661428501</v>
+        <v>11.60602258469259</v>
+      </c>
+      <c r="I15" t="n">
+        <v>56.06794928281196</v>
       </c>
     </row>
     <row r="16">
@@ -940,7 +987,7 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="E16" t="n">
         <v>804.9</v>
@@ -949,138 +996,153 @@
         <v>407.8</v>
       </c>
       <c r="G16" t="n">
-        <v>20.85973412846316</v>
+        <v>21.35669027208349</v>
       </c>
       <c r="H16" t="n">
-        <v>56.2040215792055</v>
+        <v>27.1563981042654</v>
+      </c>
+      <c r="I16" t="n">
+        <v>55.22314860225601</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>INE323A01026</t>
+          <t>INE053F01010</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>BOSCHLTD</t>
+          <t>IRFC</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Auto Components &amp; Equipments</t>
+          <t>Financial Institution</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>34451.9</v>
+        <v>153.56</v>
       </c>
       <c r="E17" t="n">
-        <v>39088.8</v>
+        <v>229</v>
       </c>
       <c r="F17" t="n">
-        <v>22133</v>
+        <v>99</v>
       </c>
       <c r="G17" t="n">
-        <v>11.86247723132969</v>
+        <v>32.94323144104803</v>
       </c>
       <c r="H17" t="n">
-        <v>55.6585189535987</v>
+        <v>49.12737692107319</v>
+      </c>
+      <c r="I17" t="n">
+        <v>55.11111111111111</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>INE053F01010</t>
+          <t>INE323A01026</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>IRFC</t>
+          <t>BOSCHLTD</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Financial Institution</t>
+          <t>Auto Components &amp; Equipments</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>153.82</v>
+        <v>34280</v>
       </c>
       <c r="E18" t="n">
-        <v>229</v>
+        <v>39088.8</v>
       </c>
       <c r="F18" t="n">
-        <v>99</v>
+        <v>22133</v>
       </c>
       <c r="G18" t="n">
-        <v>32.82969432314411</v>
+        <v>12.30224514438919</v>
       </c>
       <c r="H18" t="n">
-        <v>55.37373737373736</v>
+        <v>14.02800466744458</v>
+      </c>
+      <c r="I18" t="n">
+        <v>54.88185063028057</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>INE118A01012</t>
+          <t>INE066F01020</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>BAJAJHLDNG</t>
+          <t>HAL</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Holding Company</t>
+          <t>Aerospace &amp; Defense</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>11837.5</v>
+        <v>4203</v>
       </c>
       <c r="E19" t="n">
-        <v>13238</v>
+        <v>5674.75</v>
       </c>
       <c r="F19" t="n">
-        <v>7659.95</v>
+        <v>2763</v>
       </c>
       <c r="G19" t="n">
-        <v>10.57939265750113</v>
+        <v>25.93506321864399</v>
       </c>
       <c r="H19" t="n">
-        <v>54.53756225562832</v>
+        <v>35.0166547704021</v>
+      </c>
+      <c r="I19" t="n">
+        <v>52.11726384364821</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>INE066F01020</t>
+          <t>INE118A01012</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>HAL</t>
+          <t>BAJAJHLDNG</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Aerospace &amp; Defense</t>
+          <t>Holding Company</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>4248</v>
+        <v>11562</v>
       </c>
       <c r="E20" t="n">
-        <v>5674.75</v>
+        <v>13238</v>
       </c>
       <c r="F20" t="n">
-        <v>2763</v>
+        <v>7659.95</v>
       </c>
       <c r="G20" t="n">
-        <v>25.14207674346888</v>
+        <v>12.66052273757365</v>
       </c>
       <c r="H20" t="n">
-        <v>53.74592833876222</v>
+        <v>14.49576197889639</v>
+      </c>
+      <c r="I20" t="n">
+        <v>50.94093303481093</v>
       </c>
     </row>
     <row r="21">
@@ -1100,7 +1162,7 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>3074.45</v>
+        <v>3055</v>
       </c>
       <c r="E21" t="n">
         <v>3652.25</v>
@@ -1109,10 +1171,13 @@
         <v>2029</v>
       </c>
       <c r="G21" t="n">
-        <v>15.8203846943665</v>
+        <v>16.35293312341707</v>
       </c>
       <c r="H21" t="n">
-        <v>51.5253819615574</v>
+        <v>19.54991816693945</v>
+      </c>
+      <c r="I21" t="n">
+        <v>50.56678166584525</v>
       </c>
     </row>
     <row r="22">
@@ -1132,7 +1197,7 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>5347.45</v>
+        <v>5310</v>
       </c>
       <c r="E22" t="n">
         <v>5385.7</v>
@@ -1141,10 +1206,13 @@
         <v>3562.45</v>
       </c>
       <c r="G22" t="n">
-        <v>0.7102140854485017</v>
+        <v>1.405574020090239</v>
       </c>
       <c r="H22" t="n">
-        <v>50.10596639952843</v>
+        <v>1.425612052730685</v>
+      </c>
+      <c r="I22" t="n">
+        <v>49.05472357506773</v>
       </c>
     </row>
     <row r="23">
@@ -1164,7 +1232,7 @@
         </is>
       </c>
       <c r="D23" t="n">
-        <v>3383.35</v>
+        <v>3405</v>
       </c>
       <c r="E23" t="n">
         <v>3590.7</v>
@@ -1173,202 +1241,223 @@
         <v>2301.6</v>
       </c>
       <c r="G23" t="n">
-        <v>5.77464004233158</v>
+        <v>5.171693541649258</v>
       </c>
       <c r="H23" t="n">
-        <v>46.9999131039277</v>
+        <v>5.453744493392065</v>
+      </c>
+      <c r="I23" t="n">
+        <v>47.94056308654851</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>INE669C01036</t>
+          <t>INE726G01019</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>TECHM</t>
+          <t>ICICIPRULI</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Computers - Software &amp; Consulting</t>
+          <t>Life Insurance</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>1697</v>
+        <v>676.2</v>
       </c>
       <c r="E24" t="n">
-        <v>1807.7</v>
+        <v>796.8</v>
       </c>
       <c r="F24" t="n">
-        <v>1162.95</v>
+        <v>463.45</v>
       </c>
       <c r="G24" t="n">
-        <v>6.12380372849477</v>
+        <v>15.13554216867469</v>
       </c>
       <c r="H24" t="n">
-        <v>45.92200868481018</v>
+        <v>17.83496007098491</v>
+      </c>
+      <c r="I24" t="n">
+        <v>45.9057071960298</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>INE726G01019</t>
+          <t>INE669C01036</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>ICICIPRULI</t>
+          <t>TECHM</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Life Insurance</t>
+          <t>Computers - Software &amp; Consulting</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>671.85</v>
+        <v>1690.5</v>
       </c>
       <c r="E25" t="n">
-        <v>796.8</v>
+        <v>1807.7</v>
       </c>
       <c r="F25" t="n">
-        <v>463.45</v>
+        <v>1162.95</v>
       </c>
       <c r="G25" t="n">
-        <v>15.68147590361445</v>
+        <v>6.483376666482277</v>
       </c>
       <c r="H25" t="n">
-        <v>44.96709461646348</v>
+        <v>6.932860100561977</v>
+      </c>
+      <c r="I25" t="n">
+        <v>45.36308525731974</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>INE044A01036</t>
+          <t>INE670K01029</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>SUNPHARMA</t>
+          <t>LODHA</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Pharmaceuticals</t>
+          <t>Residential Commercial Projects</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>1857.3</v>
+        <v>1403.95</v>
       </c>
       <c r="E26" t="n">
-        <v>1960.35</v>
+        <v>1649.95</v>
       </c>
       <c r="F26" t="n">
-        <v>1287</v>
+        <v>977.35</v>
       </c>
       <c r="G26" t="n">
-        <v>5.25671436223123</v>
+        <v>14.90954271341556</v>
       </c>
       <c r="H26" t="n">
-        <v>44.31235431235432</v>
+        <v>17.52199152391467</v>
+      </c>
+      <c r="I26" t="n">
+        <v>43.64864173530465</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>INE670K01029</t>
+          <t>INE044A01036</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>LODHA</t>
+          <t>SUNPHARMA</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Residential Commercial Projects</t>
+          <t>Pharmaceuticals</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>1398.3</v>
+        <v>1848.65</v>
       </c>
       <c r="E27" t="n">
-        <v>1649.95</v>
+        <v>1960.35</v>
       </c>
       <c r="F27" t="n">
-        <v>977.35</v>
+        <v>1287</v>
       </c>
       <c r="G27" t="n">
-        <v>15.25197733264645</v>
+        <v>5.697962098604837</v>
       </c>
       <c r="H27" t="n">
-        <v>43.07054791016522</v>
+        <v>6.042247045141047</v>
+      </c>
+      <c r="I27" t="n">
+        <v>43.64024864024864</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>INE010B01027</t>
+          <t>INE009A01021</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>ZYDUSLIFE</t>
+          <t>INFY</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Pharmaceuticals</t>
+          <t>Computers - Software &amp; Consulting</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>978.85</v>
+        <v>1939.1</v>
       </c>
       <c r="E28" t="n">
-        <v>1324.3</v>
+        <v>2006.45</v>
       </c>
       <c r="F28" t="n">
-        <v>686</v>
+        <v>1358.35</v>
       </c>
       <c r="G28" t="n">
-        <v>26.08547912104508</v>
+        <v>3.356674724015063</v>
       </c>
       <c r="H28" t="n">
-        <v>42.68950437317785</v>
+        <v>3.47326079108865</v>
+      </c>
+      <c r="I28" t="n">
+        <v>42.75407663709647</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>INE009A01021</t>
+          <t>INE010B01027</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>INFY</t>
+          <t>ZYDUSLIFE</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Computers - Software &amp; Consulting</t>
+          <t>Pharmaceuticals</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>1936.75</v>
+        <v>971.75</v>
       </c>
       <c r="E29" t="n">
-        <v>2006.45</v>
+        <v>1324.3</v>
       </c>
       <c r="F29" t="n">
-        <v>1358.35</v>
+        <v>686</v>
       </c>
       <c r="G29" t="n">
-        <v>3.473797004659973</v>
+        <v>26.62161141735256</v>
       </c>
       <c r="H29" t="n">
-        <v>42.58107262487578</v>
+        <v>36.27990738358631</v>
+      </c>
+      <c r="I29" t="n">
+        <v>41.65451895043732</v>
       </c>
     </row>
     <row r="30">
@@ -1388,7 +1477,7 @@
         </is>
       </c>
       <c r="D30" t="n">
-        <v>295.95</v>
+        <v>295.2</v>
       </c>
       <c r="E30" t="n">
         <v>320</v>
@@ -1397,74 +1486,83 @@
         <v>208.5</v>
       </c>
       <c r="G30" t="n">
-        <v>7.515625000000004</v>
+        <v>7.750000000000002</v>
       </c>
       <c r="H30" t="n">
-        <v>41.94244604316546</v>
+        <v>8.401084010840121</v>
+      </c>
+      <c r="I30" t="n">
+        <v>41.58273381294963</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>INE931S01010</t>
+          <t>INE752E01010</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>ADANIENSOL</t>
+          <t>POWERGRID</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Power Distribution</t>
+          <t>Power - Transmission</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>827.4</v>
+        <v>315.8</v>
       </c>
       <c r="E31" t="n">
-        <v>1348</v>
+        <v>366.25</v>
       </c>
       <c r="F31" t="n">
-        <v>588</v>
+        <v>226.05</v>
       </c>
       <c r="G31" t="n">
-        <v>38.62017804154303</v>
+        <v>13.77474402730375</v>
       </c>
       <c r="H31" t="n">
-        <v>40.7142857142857</v>
+        <v>15.97530082330589</v>
+      </c>
+      <c r="I31" t="n">
+        <v>39.70360539703606</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>INE752E01010</t>
+          <t>INE931S01010</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>POWERGRID</t>
+          <t>ADANIENSOL</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Power - Transmission</t>
+          <t>Power Distribution</t>
         </is>
       </c>
       <c r="D32" t="n">
-        <v>316.45</v>
+        <v>821</v>
       </c>
       <c r="E32" t="n">
-        <v>366.25</v>
+        <v>1348</v>
       </c>
       <c r="F32" t="n">
-        <v>226.05</v>
+        <v>588</v>
       </c>
       <c r="G32" t="n">
-        <v>13.59726962457338</v>
+        <v>39.09495548961425</v>
       </c>
       <c r="H32" t="n">
-        <v>39.99115239991151</v>
+        <v>64.19001218026796</v>
+      </c>
+      <c r="I32" t="n">
+        <v>39.62585034013606</v>
       </c>
     </row>
     <row r="33">
@@ -1484,7 +1582,7 @@
         </is>
       </c>
       <c r="D33" t="n">
-        <v>952.55</v>
+        <v>955</v>
       </c>
       <c r="E33" t="n">
         <v>1097</v>
@@ -1493,202 +1591,223 @@
         <v>687.8</v>
       </c>
       <c r="G33" t="n">
-        <v>13.16773017319964</v>
+        <v>12.94439380127621</v>
       </c>
       <c r="H33" t="n">
-        <v>38.49229427159058</v>
+        <v>14.86910994764399</v>
+      </c>
+      <c r="I33" t="n">
+        <v>38.84850247164875</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>INE917I01010</t>
+          <t>INE200M01039</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>BAJAJ-AUTO</t>
+          <t>VBL</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>2/3 Wheelers</t>
+          <t>Other Beverages</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>9043.85</v>
+        <v>651.7</v>
       </c>
       <c r="E34" t="n">
-        <v>12774</v>
+        <v>681.12</v>
       </c>
       <c r="F34" t="n">
-        <v>6604</v>
+        <v>478.56</v>
       </c>
       <c r="G34" t="n">
-        <v>29.20111163300454</v>
+        <v>4.319356354240067</v>
       </c>
       <c r="H34" t="n">
-        <v>36.94503331314356</v>
+        <v>4.514347092220339</v>
+      </c>
+      <c r="I34" t="n">
+        <v>36.17937144767638</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>INE200M01039</t>
+          <t>INE917I01010</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>VBL</t>
+          <t>BAJAJ-AUTO</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Other Beverages</t>
+          <t>2/3 Wheelers</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>648.95</v>
+        <v>8965</v>
       </c>
       <c r="E35" t="n">
-        <v>681.12</v>
+        <v>12774</v>
       </c>
       <c r="F35" t="n">
-        <v>478.56</v>
+        <v>6604</v>
       </c>
       <c r="G35" t="n">
-        <v>4.723103124265904</v>
+        <v>29.81838108658213</v>
       </c>
       <c r="H35" t="n">
-        <v>35.60473085924441</v>
+        <v>42.48745119910764</v>
+      </c>
+      <c r="I35" t="n">
+        <v>35.75105996365839</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>INE399L01023</t>
+          <t>INE765G01017</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>ATGL</t>
+          <t>ICICIGI</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>LPG/CNG/PNG/LNG Supplier</t>
+          <t>General Insurance</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>737.45</v>
+        <v>1835</v>
       </c>
       <c r="E36" t="n">
-        <v>1190</v>
+        <v>2301.9</v>
       </c>
       <c r="F36" t="n">
-        <v>545.75</v>
+        <v>1353.5</v>
       </c>
       <c r="G36" t="n">
-        <v>38.02941176470588</v>
+        <v>20.28324427646727</v>
       </c>
       <c r="H36" t="n">
-        <v>35.12597343105818</v>
+        <v>25.4441416893733</v>
+      </c>
+      <c r="I36" t="n">
+        <v>35.57443664573328</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>INE134E01011</t>
+          <t>INE029A01011</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>PFC</t>
+          <t>BPCL</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Financial Institution</t>
+          <t>Refineries &amp; Marketing</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>469.7</v>
+        <v>296.7</v>
       </c>
       <c r="E37" t="n">
-        <v>580</v>
+        <v>376</v>
       </c>
       <c r="F37" t="n">
-        <v>351.7</v>
+        <v>222.55</v>
       </c>
       <c r="G37" t="n">
-        <v>19.01724137931035</v>
+        <v>21.09042553191489</v>
       </c>
       <c r="H37" t="n">
-        <v>33.55132214955929</v>
+        <v>26.72733400741489</v>
+      </c>
+      <c r="I37" t="n">
+        <v>33.31835542574701</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>INE765G01017</t>
+          <t>INE399L01023</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>ICICIGI</t>
+          <t>ATGL</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>General Insurance</t>
+          <t>LPG/CNG/PNG/LNG Supplier</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>1806.75</v>
+        <v>725.8</v>
       </c>
       <c r="E38" t="n">
-        <v>2301.9</v>
+        <v>1190</v>
       </c>
       <c r="F38" t="n">
-        <v>1353.5</v>
+        <v>545.75</v>
       </c>
       <c r="G38" t="n">
-        <v>21.51049133324645</v>
+        <v>39.00840336134455</v>
       </c>
       <c r="H38" t="n">
-        <v>33.48725526413003</v>
+        <v>63.95701295122625</v>
+      </c>
+      <c r="I38" t="n">
+        <v>32.99129638112688</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>INE062A01020</t>
+          <t>INE494B01023</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>SBIN</t>
+          <t>TVSMOTOR</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Public Sector Bank</t>
+          <t>2/3 Wheelers</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>799.5</v>
+        <v>2484</v>
       </c>
       <c r="E39" t="n">
-        <v>912</v>
+        <v>2958</v>
       </c>
       <c r="F39" t="n">
-        <v>600.65</v>
+        <v>1873</v>
       </c>
       <c r="G39" t="n">
-        <v>12.33552631578947</v>
+        <v>16.02434077079108</v>
       </c>
       <c r="H39" t="n">
-        <v>33.10580204778157</v>
+        <v>19.08212560386473</v>
+      </c>
+      <c r="I39" t="n">
+        <v>32.62146289375334</v>
       </c>
     </row>
     <row r="40">
@@ -1708,7 +1827,7 @@
         </is>
       </c>
       <c r="D40" t="n">
-        <v>1702.2</v>
+        <v>1694.5</v>
       </c>
       <c r="E40" t="n">
         <v>2106</v>
@@ -1717,234 +1836,223 @@
         <v>1280</v>
       </c>
       <c r="G40" t="n">
-        <v>19.17378917378917</v>
+        <v>19.53941120607787</v>
       </c>
       <c r="H40" t="n">
-        <v>32.984375</v>
+        <v>24.28444969017409</v>
+      </c>
+      <c r="I40" t="n">
+        <v>32.38281249999999</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>INE029A01011</t>
+          <t>INE134E01011</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>BPCL</t>
+          <t>PFC</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Refineries &amp; Marketing</t>
+          <t>Financial Institution</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>295.85</v>
+        <v>465</v>
       </c>
       <c r="E41" t="n">
-        <v>376</v>
+        <v>580</v>
       </c>
       <c r="F41" t="n">
-        <v>222.55</v>
+        <v>351.7</v>
       </c>
       <c r="G41" t="n">
-        <v>21.31648936170212</v>
+        <v>19.82758620689655</v>
       </c>
       <c r="H41" t="n">
-        <v>32.93641878229612</v>
+        <v>24.73118279569892</v>
+      </c>
+      <c r="I41" t="n">
+        <v>32.21495592834802</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>INE494B01023</t>
+          <t>INE062A01020</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>TVSMOTOR</t>
+          <t>SBIN</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>2/3 Wheelers</t>
+          <t>Public Sector Bank</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>2486.1</v>
+        <v>793.3</v>
       </c>
       <c r="E42" t="n">
-        <v>2958</v>
+        <v>912</v>
       </c>
       <c r="F42" t="n">
-        <v>1873</v>
+        <v>600.65</v>
       </c>
       <c r="G42" t="n">
-        <v>15.95334685598377</v>
+        <v>13.01535087719299</v>
       </c>
       <c r="H42" t="n">
-        <v>32.73358248798719</v>
+        <v>14.96281356359512</v>
+      </c>
+      <c r="I42" t="n">
+        <v>32.07358694747357</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>INE090A01021</t>
+          <t>INE020B01018</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>ICICIBANK</t>
+          <t>RECLTD</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Private Sector Bank</t>
+          <t>Financial Institution</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>1271.75</v>
+        <v>537.85</v>
       </c>
       <c r="E43" t="n">
-        <v>1362.35</v>
+        <v>654</v>
       </c>
       <c r="F43" t="n">
-        <v>970.15</v>
+        <v>408.3</v>
       </c>
       <c r="G43" t="n">
-        <v>6.650273424597197</v>
+        <v>17.75993883792049</v>
       </c>
       <c r="H43" t="n">
-        <v>31.08797608617224</v>
+        <v>21.59524030863622</v>
+      </c>
+      <c r="I43" t="n">
+        <v>31.72912074455059</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>INE121A01024</t>
+          <t>INE758E01017</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>CHOLAFIN</t>
+          <t>JIOFIN</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Non Banking Financial Company (NBFC)</t>
+          <t>Investment Company</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>1325.55</v>
+        <v>307.15</v>
       </c>
       <c r="E44" t="n">
-        <v>1652</v>
+        <v>394.7</v>
       </c>
       <c r="F44" t="n">
-        <v>1011.2</v>
+        <v>233.55</v>
       </c>
       <c r="G44" t="n">
-        <v>19.76089588377724</v>
+        <v>22.18140359766912</v>
       </c>
       <c r="H44" t="n">
-        <v>31.08682753164555</v>
+        <v>28.50398827934235</v>
+      </c>
+      <c r="I44" t="n">
+        <v>31.51359451937486</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>INE758E01017</t>
+          <t>INE090A01021</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>JIOFIN</t>
+          <t>ICICIBANK</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Investment Company</t>
+          <t>Private Sector Bank</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>305.95</v>
+        <v>1265.6</v>
       </c>
       <c r="E45" t="n">
-        <v>394.7</v>
+        <v>1362.35</v>
       </c>
       <c r="F45" t="n">
-        <v>233.55</v>
+        <v>970.15</v>
       </c>
       <c r="G45" t="n">
-        <v>22.48543197365087</v>
+        <v>7.101699269644368</v>
       </c>
       <c r="H45" t="n">
-        <v>30.9997859130807</v>
+        <v>7.644595448798985</v>
+      </c>
+      <c r="I45" t="n">
+        <v>30.45405349688193</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>INE020B01018</t>
+          <t>INE121A01024</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>RECLTD</t>
+          <t>CHOLAFIN</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Financial Institution</t>
+          <t>Non Banking Financial Company (NBFC)</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>534.5</v>
+        <v>1315.9</v>
       </c>
       <c r="E46" t="n">
-        <v>654</v>
+        <v>1652</v>
       </c>
       <c r="F46" t="n">
-        <v>408.3</v>
+        <v>1011.2</v>
       </c>
       <c r="G46" t="n">
-        <v>18.27217125382263</v>
+        <v>20.34503631961259</v>
       </c>
       <c r="H46" t="n">
-        <v>30.90864560372275</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="inlineStr">
-        <is>
-          <t>INE437A01024</t>
-        </is>
-      </c>
-      <c r="B47" t="inlineStr">
-        <is>
-          <t>APOLLOHOSP</t>
-        </is>
-      </c>
-      <c r="C47" t="inlineStr">
-        <is>
-          <t>Hospital</t>
-        </is>
-      </c>
-      <c r="D47" t="n">
-        <v>7363.95</v>
-      </c>
-      <c r="E47" t="n">
-        <v>7545</v>
-      </c>
-      <c r="F47" t="n">
-        <v>5640</v>
-      </c>
-      <c r="G47" t="n">
-        <v>2.399602385685884</v>
-      </c>
-      <c r="H47" t="n">
-        <v>30.56648936170212</v>
+        <v>25.5414545178205</v>
+      </c>
+      <c r="I46" t="n">
+        <v>30.13251582278482</v>
       </c>
     </row>
   </sheetData>

</xml_diff>